<commit_message>
Code updated for 4 problem
Code updated for 4 problem
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927A05F9-3163-4EFB-B6EC-12C5DD808E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75E0AF6-55B4-45D1-8F21-16F41E6AAE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Question No</t>
   </si>
@@ -94,6 +94,21 @@
       </rPr>
       <t>2. Recursive Approach:-</t>
     </r>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Implement Lower Bound</t>
+  </si>
+  <si>
+    <t>Implement Upper Bound</t>
+  </si>
+  <si>
+    <t>Search Insert Position</t>
+  </si>
+  <si>
+    <t>Ceil the floor</t>
   </si>
 </sst>
 </file>
@@ -501,20 +516,20 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="59.7109375" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="70.44140625" customWidth="1"/>
+    <col min="4" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="59.6640625" customWidth="1"/>
+    <col min="7" max="7" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -537,7 +552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>704</v>
       </c>
@@ -557,27 +572,73 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+    <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -585,7 +646,7 @@
       <c r="E7"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="D8" s="1"/>
@@ -593,7 +654,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
@@ -601,21 +662,21 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12"/>
@@ -623,62 +684,62 @@
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
@@ -686,11 +747,11 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -698,61 +759,61 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
540.  Single element in a Sorted Array
540.  Single element in a Sorted Array
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EE6620-F513-46C8-9967-B22BB82F86C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C01EF1-1F33-4421-B28A-98C1F8DE6DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Question No</t>
   </si>
@@ -331,6 +331,15 @@
       <t xml:space="preserve">
 (Accordingly if the element is in left or right half of the mid we will adjust high and low)</t>
     </r>
+  </si>
+  <si>
+    <t>CN/LC</t>
+  </si>
+  <si>
+    <t>Single Element in a Sorted Array</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -369,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +400,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -478,6 +493,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,21 +780,21 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="70.44140625" style="16" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="59.6640625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="12.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" style="16" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="59.7109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>704</v>
       </c>
@@ -819,7 +837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>12</v>
@@ -837,7 +855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>12</v>
@@ -855,7 +873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>35</v>
       </c>
@@ -873,7 +891,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -891,15 +909,25 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>540</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="D8" s="7"/>
@@ -907,7 +935,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
@@ -915,21 +943,21 @@
       <c r="E9" s="5"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="5"/>
       <c r="C12" s="16"/>
@@ -937,62 +965,62 @@
       <c r="E12" s="7"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="5"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="18"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="18"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="18"/>
       <c r="D23" s="7"/>
@@ -1000,11 +1028,11 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="18"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="5"/>
       <c r="C25" s="18"/>
@@ -1012,65 +1040,68 @@
       <c r="E25" s="7"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="18"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="18"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="18"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="21"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="21"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="21"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="C37" s="21"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="21"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" display="https://leetcode.com/problems/single-element-in-a-sorted-array/" xr:uid="{2B8FED24-D557-4320-9F9E-3F853414AC69}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code of many probleme and excel sheet
updated code of many probleme and excel sheet
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C01EF1-1F33-4421-B28A-98C1F8DE6DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C5D9A5-41C6-4E46-BBAF-B133B4572CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>Question No</t>
   </si>
@@ -340,6 +340,78 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>Find Peak Element</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Sorted Array</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Number of occurrence-
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sheet </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Count Occurrences in Sorted Array</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rotation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sheet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Find out how many times the array has been rotated</t>
+    </r>
+  </si>
+  <si>
+    <t>Search Element in a Rotated Sorted Array - I</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array II</t>
   </si>
 </sst>
 </file>
@@ -777,24 +849,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" style="16" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="59.7109375" style="16" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="12.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="70.44140625" style="16" customWidth="1"/>
+    <col min="4" max="5" width="17.88671875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="59.6640625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="43.109375" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>704</v>
       </c>
@@ -837,7 +909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>12</v>
@@ -855,7 +927,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>12</v>
@@ -873,7 +945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>35</v>
       </c>
@@ -891,7 +963,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -909,15 +981,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>540</v>
+        <v>34</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>6</v>
@@ -927,181 +999,291 @@
       </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F8" s="18"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+    </row>
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>81</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>153</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>540</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>162</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
       <c r="B17" s="5"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
       <c r="B18" s="5"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="5"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="18"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
-      <c r="C23" s="18"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="18"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="18"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="18"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="18"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="C30" s="18"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
       <c r="B31" s="5"/>
       <c r="C31" s="18"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="18"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="C34" s="21"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
-      <c r="C35" s="21"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
-      <c r="C36" s="21"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="21"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="18"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="21"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="18"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
       <c r="B39" s="5"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
+      <c r="C40" s="21"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="5"/>
+      <c r="C41" s="21"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="5"/>
+      <c r="C42" s="21"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="5"/>
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="5"/>
+      <c r="C44" s="21"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" display="https://leetcode.com/problems/single-element-in-a-sorted-array/" xr:uid="{2B8FED24-D557-4320-9F9E-3F853414AC69}"/>
+    <hyperlink ref="C13" r:id="rId1" display="https://leetcode.com/problems/single-element-in-a-sorted-array/" xr:uid="{2B8FED24-D557-4320-9F9E-3F853414AC69}"/>
+    <hyperlink ref="C14" r:id="rId2" display="https://leetcode.com/problems/find-peak-element/" xr:uid="{87678BFB-36D5-415A-B081-5DE8D85E7E18}"/>
+    <hyperlink ref="C7" r:id="rId3" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array/" xr:uid="{519AFF46-875B-4229-9DEB-89142F56F32E}"/>
+    <hyperlink ref="C11" r:id="rId4" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/" xr:uid="{F8973700-DFD3-4D54-8116-C974B27B1342}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Coding Ninja - Finding Square root of a number
Coding Ninja - Finding Square root of a number
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C5D9A5-41C6-4E46-BBAF-B133B4572CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156CD4C1-74A4-4DBB-B456-62B8A08E5E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Question No</t>
   </si>
@@ -412,6 +412,59 @@
   </si>
   <si>
     <t>Search in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>CN/GFG</t>
+  </si>
+  <si>
+    <t>Finding Sqrt of a number using Binary Search</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. Naïve Approach :-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+We will iterate till the number in for loop and check if square of i is less than N.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. Binary Search :-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -509,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -568,6 +621,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,21 +908,21 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="70.44140625" style="16" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="59.6640625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="12.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" style="16" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="59.7109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>704</v>
       </c>
@@ -909,7 +965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>12</v>
@@ -927,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>12</v>
@@ -945,7 +1001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>35</v>
       </c>
@@ -963,7 +1019,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -981,7 +1037,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>34</v>
       </c>
@@ -999,7 +1055,7 @@
       </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>12</v>
@@ -1015,13 +1071,11 @@
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>33</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="9" t="s">
         <v>29</v>
       </c>
@@ -1033,7 +1087,7 @@
       </c>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>81</v>
       </c>
@@ -1051,7 +1105,7 @@
       </c>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>153</v>
       </c>
@@ -1069,7 +1123,7 @@
       </c>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>12</v>
@@ -1085,7 +1139,7 @@
       </c>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>540</v>
       </c>
@@ -1103,7 +1157,7 @@
       </c>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>162</v>
       </c>
@@ -1122,21 +1176,38 @@
       <c r="F14" s="18"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="5"/>
       <c r="C18" s="16"/>
@@ -1144,62 +1215,62 @@
       <c r="E18" s="7"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="5"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="18"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="18"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="18"/>
       <c r="D29" s="7"/>
@@ -1207,11 +1278,11 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="18"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
       <c r="B31" s="5"/>
       <c r="C31" s="18"/>
@@ -1219,61 +1290,61 @@
       <c r="E31" s="7"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="18"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="18"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="18"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="21"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="21"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="21"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="21"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="21"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Coding Ninja -  Find the Nth root of an Integer
Coding Ninja -  Find the Nth root of an Integer
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156CD4C1-74A4-4DBB-B456-62B8A08E5E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A009BA5-4120-4769-926D-1913F19B115B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Question No</t>
   </si>
@@ -464,6 +464,48 @@
       </rPr>
       <t xml:space="preserve">
 </t>
+    </r>
+  </si>
+  <si>
+    <t>Find the Nth root of an Integer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Naïve Approach :-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+We will iterate till the number in for loop and check if square of i is less than </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N.
+2. Binary Search :-</t>
     </r>
   </si>
 </sst>
@@ -562,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -622,8 +664,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,7 +978,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +987,7 @@
     <col min="2" max="2" width="20.42578125" style="17" customWidth="1"/>
     <col min="3" max="3" width="70.42578125" style="16" customWidth="1"/>
     <col min="4" max="5" width="17.85546875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="59.7109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" style="16" customWidth="1"/>
     <col min="7" max="7" width="43.140625" style="16" customWidth="1"/>
     <col min="8" max="16384" width="8.85546875" style="16"/>
   </cols>
@@ -1176,29 +1246,41 @@
       <c r="F14" s="18"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+    <row r="15" spans="1:7" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="18"/>
+    <row r="16" spans="1:7" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
@@ -1207,13 +1289,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="18"/>
+    <row r="18" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>

</xml_diff>

<commit_message>
875. Koko eating Bananas
875. Koko eating Bananas
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A009BA5-4120-4769-926D-1913F19B115B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485BDDF7-6551-415E-8EDA-C093B3933BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>Question No</t>
   </si>
@@ -507,6 +507,9 @@
       <t>N.
 2. Binary Search :-</t>
     </r>
+  </si>
+  <si>
+    <t>Koko Eating Bananas</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -680,19 +683,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -977,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,18 +1273,28 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="A17" s="5">
+        <v>875</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
@@ -1434,8 +1434,9 @@
     <hyperlink ref="C14" r:id="rId2" display="https://leetcode.com/problems/find-peak-element/" xr:uid="{87678BFB-36D5-415A-B081-5DE8D85E7E18}"/>
     <hyperlink ref="C7" r:id="rId3" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array/" xr:uid="{519AFF46-875B-4229-9DEB-89142F56F32E}"/>
     <hyperlink ref="C11" r:id="rId4" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/" xr:uid="{F8973700-DFD3-4D54-8116-C974B27B1342}"/>
+    <hyperlink ref="C17" r:id="rId5" display="https://leetcode.com/problems/koko-eating-bananas/" xr:uid="{0185A566-ABC0-4D21-B45C-59281DBFFD49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1482. Minimum Number of Days to make m Bouquets
1482. Minimum Number of Days to make m Bouquets
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485BDDF7-6551-415E-8EDA-C093B3933BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D09045-38A6-401B-9361-9B5FEBA55510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>Question No</t>
   </si>
@@ -510,6 +510,12 @@
   </si>
   <si>
     <t>Koko Eating Bananas</t>
+  </si>
+  <si>
+    <t>Minimum Number of Days to Make m Bouquets</t>
+  </si>
+  <si>
+    <t>1. Use Binary search and find the minimum day on which you can make certain number of boq with fixed adjacent flower. Same as Koko eating banana</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -576,6 +582,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -685,6 +697,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,7 +990,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,29 +1294,43 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
         <v>875</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="18"/>
+      <c r="F17" s="31"/>
+    </row>
+    <row r="18" spans="1:7" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>1482</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>

</xml_diff>

<commit_message>
1283. Find the Smallest Divisor Given a Threshold
1283. Find the Smallest Divisor Given a Threshold
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D09045-38A6-401B-9361-9B5FEBA55510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A76273D-122E-4FD0-B6A9-39847716F359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t>Question No</t>
   </si>
@@ -516,6 +516,12 @@
   </si>
   <si>
     <t>1. Use Binary search and find the minimum day on which you can make certain number of boq with fixed adjacent flower. Same as Koko eating banana</t>
+  </si>
+  <si>
+    <t>Find the Smallest Divisor Given a Threshold</t>
+  </si>
+  <si>
+    <t>CN/LC/GFG</t>
   </si>
 </sst>
 </file>
@@ -989,22 +995,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" style="16" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="68.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="12.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="70.44140625" style="16" customWidth="1"/>
+    <col min="4" max="5" width="17.88671875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="68.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="43.109375" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>704</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>12</v>
@@ -1065,7 +1071,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>12</v>
@@ -1083,7 +1089,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>35</v>
       </c>
@@ -1101,7 +1107,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -1119,7 +1125,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>34</v>
       </c>
@@ -1137,7 +1143,7 @@
       </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>12</v>
@@ -1153,7 +1159,7 @@
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>33</v>
       </c>
@@ -1169,7 +1175,7 @@
       </c>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>81</v>
       </c>
@@ -1187,7 +1193,7 @@
       </c>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>153</v>
       </c>
@@ -1205,7 +1211,7 @@
       </c>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>12</v>
@@ -1221,7 +1227,7 @@
       </c>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>540</v>
       </c>
@@ -1239,7 +1245,7 @@
       </c>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>162</v>
       </c>
@@ -1258,7 +1264,7 @@
       <c r="F14" s="18"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="19" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="23"/>
       <c r="B15" s="24" t="s">
         <v>31</v>
@@ -1276,7 +1282,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="27"/>
       <c r="B16" s="27" t="s">
         <v>31</v>
@@ -1294,7 +1300,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29">
         <v>875</v>
       </c>
@@ -1307,12 +1313,12 @@
       <c r="D17" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="31"/>
     </row>
-    <row r="18" spans="1:7" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="32" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>1482</v>
       </c>
@@ -1325,69 +1331,81 @@
       <c r="D18" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29">
+        <v>1283</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="18"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="18"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="18"/>
       <c r="D29" s="7"/>
@@ -1395,11 +1413,11 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="18"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="20"/>
       <c r="B31" s="5"/>
       <c r="C31" s="18"/>
@@ -1407,61 +1425,61 @@
       <c r="E31" s="7"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="18"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="18"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="18"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
       <c r="C40" s="21"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="5"/>
       <c r="C41" s="21"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="5"/>
       <c r="C42" s="21"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="5"/>
       <c r="C43" s="21"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="5"/>
       <c r="C44" s="21"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
     </row>
   </sheetData>
@@ -1471,8 +1489,9 @@
     <hyperlink ref="C7" r:id="rId3" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array/" xr:uid="{519AFF46-875B-4229-9DEB-89142F56F32E}"/>
     <hyperlink ref="C11" r:id="rId4" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/" xr:uid="{F8973700-DFD3-4D54-8116-C974B27B1342}"/>
     <hyperlink ref="C17" r:id="rId5" display="https://leetcode.com/problems/koko-eating-bananas/" xr:uid="{0185A566-ABC0-4D21-B45C-59281DBFFD49}"/>
+    <hyperlink ref="C19" r:id="rId6" display="https://leetcode.com/problems/find-the-smallest-divisor-given-a-threshold/" xr:uid="{4E4E42DD-BD4F-48D2-929C-6A74BAFA41D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1011. Capacity To Ship Packages Within D Days
1011. Capacity To Ship Packages Within D Days
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A76273D-122E-4FD0-B6A9-39847716F359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7DC430-4DCF-4CCF-AE5E-2013B2D85A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t>Question No</t>
   </si>
@@ -522,6 +522,9 @@
   </si>
   <si>
     <t>CN/LC/GFG</t>
+  </si>
+  <si>
+    <t>Capacity To Ship Packages Within D Days</t>
   </si>
 </sst>
 </file>
@@ -995,22 +998,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="70.44140625" style="16" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="68.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="12.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" style="16" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>704</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>12</v>
@@ -1071,7 +1074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>12</v>
@@ -1089,7 +1092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>35</v>
       </c>
@@ -1107,7 +1110,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -1125,7 +1128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>34</v>
       </c>
@@ -1143,7 +1146,7 @@
       </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>12</v>
@@ -1159,7 +1162,7 @@
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>33</v>
       </c>
@@ -1175,7 +1178,7 @@
       </c>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>81</v>
       </c>
@@ -1193,7 +1196,7 @@
       </c>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>153</v>
       </c>
@@ -1211,7 +1214,7 @@
       </c>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>12</v>
@@ -1227,7 +1230,7 @@
       </c>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>540</v>
       </c>
@@ -1245,7 +1248,7 @@
       </c>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>162</v>
       </c>
@@ -1264,7 +1267,7 @@
       <c r="F14" s="18"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" s="19" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="24" t="s">
         <v>31</v>
@@ -1282,7 +1285,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="27" t="s">
         <v>31</v>
@@ -1300,7 +1303,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>875</v>
       </c>
@@ -1318,7 +1321,7 @@
       </c>
       <c r="F17" s="31"/>
     </row>
-    <row r="18" spans="1:7" s="32" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>1482</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>1283</v>
       </c>
@@ -1356,56 +1359,69 @@
       </c>
       <c r="F19" s="31"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <v>1011</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="18"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="18"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="18"/>
       <c r="D29" s="7"/>
@@ -1413,11 +1429,11 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="18"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
       <c r="B31" s="5"/>
       <c r="C31" s="18"/>
@@ -1425,61 +1441,61 @@
       <c r="E31" s="7"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="18"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="18"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="18"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="21"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="21"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="21"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="21"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="21"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
     </row>
   </sheetData>
@@ -1490,8 +1506,9 @@
     <hyperlink ref="C11" r:id="rId4" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/" xr:uid="{F8973700-DFD3-4D54-8116-C974B27B1342}"/>
     <hyperlink ref="C17" r:id="rId5" display="https://leetcode.com/problems/koko-eating-bananas/" xr:uid="{0185A566-ABC0-4D21-B45C-59281DBFFD49}"/>
     <hyperlink ref="C19" r:id="rId6" display="https://leetcode.com/problems/find-the-smallest-divisor-given-a-threshold/" xr:uid="{4E4E42DD-BD4F-48D2-929C-6A74BAFA41D5}"/>
+    <hyperlink ref="C20" r:id="rId7" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days/" xr:uid="{0B66FD97-4574-4866-8AAD-AC1543C605C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Coding ninja - Aggressive cows
Coding ninja - Aggressive cows
</commit_message>
<xml_diff>
--- a/Binary Search/Question_List-Java version.xlsx
+++ b/Binary Search/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\GIT\Leetcode\Binary Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7DC430-4DCF-4CCF-AE5E-2013B2D85A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C320E23-6ACA-483D-B36C-6B646E2DB703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
   <si>
     <t>Question No</t>
   </si>
@@ -525,6 +525,12 @@
   </si>
   <si>
     <t>Capacity To Ship Packages Within D Days</t>
+  </si>
+  <si>
+    <t>Aggressive Cow</t>
+  </si>
+  <si>
+    <t>To find min distance which is maximum</t>
   </si>
 </sst>
 </file>
@@ -999,7 +1005,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,10 +1385,21 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>

</xml_diff>